<commit_message>
Processed 2025 TEMPEST sulfide data
</commit_message>
<xml_diff>
--- a/processing_scripts/Sulfide/Raw Data/2025_TEMPEST_H2S_Datasheets.xlsx
+++ b/processing_scripts/Sulfide/Raw Data/2025_TEMPEST_H2S_Datasheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sinet-my.sharepoint.com/personal/readz_si_edu1/Documents/TEMPEST_Porewater/processing_scripts/Sulfide/Raw Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="442" documentId="13_ncr:1_{92021526-6563-4582-BD6D-EF31E3B89D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81C23E53-D1F4-437B-863B-7033437E5F12}"/>
+  <xr:revisionPtr revIDLastSave="448" documentId="13_ncr:1_{92021526-6563-4582-BD6D-EF31E3B89D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2B5D204-30C4-424D-A202-46EBCFAABBBD}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{23FB6DB2-3641-4E78-A68E-113D11F8B05A}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{23FB6DB2-3641-4E78-A68E-113D11F8B05A}"/>
   </bookViews>
   <sheets>
     <sheet name="Plate 8" sheetId="3" r:id="rId1"/>
@@ -5184,8 +5184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C102C732-A95C-46A8-94F7-F26F268F4BF5}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5359,13 +5359,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E5" s="5">
         <v>143</v>
@@ -5401,13 +5401,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E6" s="5">
         <v>144</v>
@@ -5949,7 +5949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74CE3F3C-98FB-415A-A3A7-BEE44D11C516}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>

</xml_diff>